<commit_message>
fin du dossier excel ultra chiant et inutile sa mère
</commit_message>
<xml_diff>
--- a/Fichiers Simulations Carte SUIVI-20250411/c'est ce fichier qui marche, les autres je ne sais pas à quoi ils servent.xlsx
+++ b/Fichiers Simulations Carte SUIVI-20250411/c'est ce fichier qui marche, les autres je ne sais pas à quoi ils servent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="F1" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t xml:space="preserve">a) Ouvrir (open) le schéma oscillateur, copier votre montage oscillateur</t>
   </si>
@@ -36,6 +36,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">et venir le coller dans le rectangle de la fonction F1 </t>
     </r>
@@ -46,6 +47,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">supprimer avant le générateur de l'etude F2</t>
     </r>
@@ -295,6 +297,9 @@
   </si>
   <si>
     <t xml:space="preserve">Comment ne laisser passer sans les atténuer uniquement les composantes du signal V Sortie Capteur de fréquence &gt; 2000 Hz ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtre passe haut</t>
   </si>
   <si>
     <t xml:space="preserve">Proposez un schéma</t>
@@ -345,6 +350,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">La tension précédente n'est pas encore optimale</t>
     </r>
@@ -353,6 +359,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">; il faut rajouter une fonction qui va la transformer pour que ces caractéristiques correspondent au cahier des charges</t>
     </r>
@@ -378,12 +385,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -406,12 +414,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -419,30 +422,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -487,36 +480,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,169 +640,169 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="135.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="135.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>2.2E-008</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">0.693*(C5+C7)*C8</f>
         <v>0</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <f aca="false">0.693*C8*C7</f>
         <v>0</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -839,106 +828,106 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="70.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -960,194 +949,194 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="78.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>820</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>2.2</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>4350</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1170,74 +1159,77 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="101.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="101.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>84</v>
+      <c r="A3" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>85</v>
+      <c r="A4" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>86</v>
+      <c r="A5" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>87</v>
+      <c r="A6" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="0" t="s">
-        <v>92</v>
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>93</v>
+      <c r="A10" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1265,26 +1257,26 @@
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>94</v>
+      <c r="A1" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>95</v>
+      <c r="A2" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>96</v>
+      <c r="A3" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>97</v>
+      <c r="A5" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1305,35 +1297,35 @@
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>98</v>
+      <c r="A1" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>99</v>
+      <c r="A2" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>100</v>
+      <c r="A3" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>101</v>
+      <c r="A4" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>102</v>
+      <c r="A5" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>